<commit_message>
get data to home page
</commit_message>
<xml_diff>
--- a/ShoppingOnline/wwwroot/uploaded/excels/ProductImportTemplate.xlsx
+++ b/ShoppingOnline/wwwroot/uploaded/excels/ProductImportTemplate.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tuana\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tuana\OneDrive\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{A7576358-E4E9-466F-8732-457F6EB5CFAD}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72FC26F7-9F9F-42E5-A2B8-E6C464D30BA5}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
   <si>
     <t>Description</t>
   </si>
@@ -42,9 +42,6 @@
     <t>Original Price</t>
   </si>
   <si>
-    <t>Content</t>
-  </si>
-  <si>
     <t>Seo Keywords</t>
   </si>
   <si>
@@ -60,10 +57,10 @@
     <t>Home Flag</t>
   </si>
   <si>
-    <t>test ip1</t>
-  </si>
-  <si>
-    <t>test ip2</t>
+    <t>test</t>
+  </si>
+  <si>
+    <t>11</t>
   </si>
 </sst>
 </file>
@@ -127,7 +124,7 @@
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Original Price"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Price"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Promotion Price"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Content"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="11"/>
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Seo Keywords"/>
     <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Seo Description"/>
     <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Status"/>
@@ -404,7 +401,7 @@
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N21" sqref="N21"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -439,30 +436,30 @@
         <v>3</v>
       </c>
       <c r="F1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
         <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>10</v>
-      </c>
-      <c r="K1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -474,13 +471,13 @@
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I2">
         <v>1</v>
@@ -493,37 +490,19 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" t="s">
-        <v>12</v>
+      <c r="A3">
+        <v>111111</v>
+      </c>
+      <c r="B3">
+        <v>111</v>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="D3">
-        <v>2</v>
-      </c>
-      <c r="E3">
-        <v>12</v>
-      </c>
-      <c r="F3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
-      <c r="J3">
-        <v>1</v>
-      </c>
-      <c r="K3">
+        <v>11</v>
+      </c>
+      <c r="G3">
         <v>1</v>
       </c>
     </row>

</xml_diff>